<commit_message>
RNAsep1 assembly output (6 samples)
</commit_message>
<xml_diff>
--- a/Bioinformatics/Samples_RNAsep2.xlsx
+++ b/Bioinformatics/Samples_RNAsep2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsoldo01/Documents/Recherche/rnasep/Bioinformatics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6457A26-09DD-A84E-B830-09657072BEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6455EE9-54D3-7B44-B8D5-A2CA8A23299B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="101">
   <si>
     <t>Conditions</t>
   </si>
@@ -326,6 +326,9 @@
   </si>
   <si>
     <t>Hg8.1</t>
+  </si>
+  <si>
+    <t>Sampled used for de novo assembly</t>
   </si>
 </sst>
 </file>
@@ -366,12 +369,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -466,7 +475,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -479,6 +488,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1176,20 +1187,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="4" width="11" style="10"/>
     <col min="5" max="5" width="19.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11" style="10"/>
+    <col min="6" max="6" width="11" style="10"/>
+    <col min="7" max="7" width="29.83203125" style="10" customWidth="1"/>
+    <col min="8" max="16384" width="11" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
@@ -1207,43 +1220,46 @@
       </c>
       <c r="F1"/>
     </row>
-    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="12">
         <v>7</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="12" t="s">
         <v>67</v>
       </c>
       <c r="F2"/>
-    </row>
-    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="G2" s="12" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="12">
         <v>7</v>
       </c>
-      <c r="E3" s="10" t="s">
+      <c r="E3" s="12" t="s">
         <v>68</v>
       </c>
       <c r="F3"/>
     </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>10</v>
       </c>
@@ -1261,7 +1277,7 @@
       </c>
       <c r="F4"/>
     </row>
-    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
@@ -1279,7 +1295,7 @@
       </c>
       <c r="F5"/>
     </row>
-    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
@@ -1297,25 +1313,25 @@
       </c>
       <c r="F6"/>
     </row>
-    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="12">
         <v>7</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="12" t="s">
         <v>72</v>
       </c>
       <c r="F7"/>
     </row>
-    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
@@ -1333,25 +1349,25 @@
       </c>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="12">
         <v>7</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="12" t="s">
         <v>74</v>
       </c>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
         <v>16</v>
       </c>
@@ -1369,25 +1385,25 @@
       </c>
       <c r="F10"/>
     </row>
-    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D11" s="10">
+      <c r="D11" s="12">
         <v>8</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="12" t="s">
         <v>76</v>
       </c>
       <c r="F11"/>
     </row>
-    <row r="12" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>18</v>
       </c>
@@ -1405,43 +1421,43 @@
       </c>
       <c r="F12"/>
     </row>
-    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D13" s="10">
+      <c r="D13" s="12">
         <v>8</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="12" t="s">
         <v>78</v>
       </c>
       <c r="F13"/>
     </row>
-    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="10">
+      <c r="D14" s="12">
         <v>8</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="12" t="s">
         <v>79</v>
       </c>
       <c r="F14"/>
     </row>
-    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>21</v>
       </c>
@@ -1459,20 +1475,20 @@
       </c>
       <c r="F15"/>
     </row>
-    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="12">
         <v>8</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="12" t="s">
         <v>81</v>
       </c>
       <c r="F16"/>
@@ -1514,19 +1530,19 @@
       <c r="F18"/>
     </row>
     <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="12">
         <v>7</v>
       </c>
-      <c r="E19" s="10" t="s">
+      <c r="E19" s="12" t="s">
         <v>84</v>
       </c>
       <c r="F19"/>
@@ -1550,37 +1566,37 @@
       <c r="F20"/>
     </row>
     <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="B21" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="12">
         <v>7</v>
       </c>
-      <c r="E21" s="10" t="s">
+      <c r="E21" s="12" t="s">
         <v>86</v>
       </c>
       <c r="F21"/>
     </row>
     <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="10" t="s">
+      <c r="C22" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="12">
         <v>7</v>
       </c>
-      <c r="E22" s="10" t="s">
+      <c r="E22" s="12" t="s">
         <v>87</v>
       </c>
       <c r="F22"/>
@@ -1604,55 +1620,55 @@
       <c r="F23"/>
     </row>
     <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D24" s="12">
         <v>7</v>
       </c>
-      <c r="E24" s="10" t="s">
+      <c r="E24" s="12" t="s">
         <v>89</v>
       </c>
       <c r="F24"/>
     </row>
     <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="C25" s="10" t="s">
+      <c r="C25" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D25" s="12">
         <v>8</v>
       </c>
-      <c r="E25" s="10" t="s">
+      <c r="E25" s="12" t="s">
         <v>90</v>
       </c>
       <c r="F25"/>
     </row>
     <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="10" t="s">
+      <c r="C26" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D26" s="12">
         <v>8</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="12" t="s">
         <v>91</v>
       </c>
       <c r="F26"/>
@@ -1676,37 +1692,37 @@
       <c r="F27"/>
     </row>
     <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="12" t="s">
         <v>63</v>
       </c>
-      <c r="C28" s="10" t="s">
+      <c r="C28" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D28" s="12">
         <v>8</v>
       </c>
-      <c r="E28" s="10" t="s">
+      <c r="E28" s="12" t="s">
         <v>93</v>
       </c>
       <c r="F28"/>
     </row>
     <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="B29" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="C29" s="10" t="s">
+      <c r="C29" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D29" s="12">
         <v>8</v>
       </c>
-      <c r="E29" s="10" t="s">
+      <c r="E29" s="12" t="s">
         <v>94</v>
       </c>
       <c r="F29"/>

</xml_diff>

<commit_message>
updating modified files from Ranalysis project.
</commit_message>
<xml_diff>
--- a/Bioinformatics/Samples_RNAsep2.xlsx
+++ b/Bioinformatics/Samples_RNAsep2.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tsoldo01/Documents/Recherche/rnasep/Bioinformatics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD25994-5EE6-F14E-9DDC-6A707A7AC528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E361E646-7507-2947-9199-DD2C41A47D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="10000" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18320" yWindow="-22140" windowWidth="23240" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="SampleName" sheetId="2" r:id="rId2"/>
+    <sheet name="SampleName" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" iterateDelta="1E-4"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="138">
   <si>
     <t>Conditions</t>
   </si>
@@ -313,9 +313,6 @@
     <t>SEP2-Hg8.1_68</t>
   </si>
   <si>
-    <t>Bioinfo_SampleName</t>
-  </si>
-  <si>
     <t>CT7.7</t>
   </si>
   <si>
@@ -328,7 +325,121 @@
     <t>Hg8.1</t>
   </si>
   <si>
-    <t>Sampled used for de novo assembly</t>
+    <t>Samples used for de novo assembly</t>
+  </si>
+  <si>
+    <t>FALSE_Bioinfo_SampleName</t>
+  </si>
+  <si>
+    <t>TRUE_Bioinfo_SampleName</t>
+  </si>
+  <si>
+    <t>SEP2-CT8.1_5</t>
+  </si>
+  <si>
+    <t>SEP2-CT8.1_6</t>
+  </si>
+  <si>
+    <t>SEP2-CT8.1_8</t>
+  </si>
+  <si>
+    <t>SEP2-CT8.1_9</t>
+  </si>
+  <si>
+    <t>SEP2-CT8.1_37</t>
+  </si>
+  <si>
+    <t>SEP2-CT8.1_38</t>
+  </si>
+  <si>
+    <t>SEP2-CT8.1_39</t>
+  </si>
+  <si>
+    <t>SEP2-CT8.1_80</t>
+  </si>
+  <si>
+    <t>SEP2-CT7.7_10</t>
+  </si>
+  <si>
+    <t>SEP2-CT7.7_11</t>
+  </si>
+  <si>
+    <t>SEP2-CT7.7_12</t>
+  </si>
+  <si>
+    <t>SEP2-CT7.7_13</t>
+  </si>
+  <si>
+    <t>SEP2-CT7.7_46</t>
+  </si>
+  <si>
+    <t>SEP2-CT7.7_48</t>
+  </si>
+  <si>
+    <t>SEP2-CT7.7_85</t>
+  </si>
+  <si>
+    <t>SEP2-CT7.7_86</t>
+  </si>
+  <si>
+    <t>SEP2-Hg8.1_19</t>
+  </si>
+  <si>
+    <t>SEP2-Hg8.1_20</t>
+  </si>
+  <si>
+    <t>SEP2-Hg8.1_21</t>
+  </si>
+  <si>
+    <t>SEP2-Hg8.1_24</t>
+  </si>
+  <si>
+    <t>SEP2-Hg8.1_25</t>
+  </si>
+  <si>
+    <t>SEP2-Hg8.1_55</t>
+  </si>
+  <si>
+    <t>SEP2-Hg8.1_56</t>
+  </si>
+  <si>
+    <t>SEP2-Hg7.7_28</t>
+  </si>
+  <si>
+    <t>SEP2-Hg7.7_30</t>
+  </si>
+  <si>
+    <t>SEP2-Hg7.7_31</t>
+  </si>
+  <si>
+    <t>SEP2-Hg7.7_32</t>
+  </si>
+  <si>
+    <t>SEP2-Hg7.7_68</t>
+  </si>
+  <si>
+    <t>Treatment</t>
+  </si>
+  <si>
+    <t>Hg+CO2</t>
+  </si>
+  <si>
+    <t>Hg+CO3</t>
+  </si>
+  <si>
+    <t>Hg+CO4</t>
+  </si>
+  <si>
+    <t>Hg+CO5</t>
+  </si>
+  <si>
+    <t>Hg+CO6</t>
+  </si>
+  <si>
+    <t>8.1</t>
+  </si>
+  <si>
+    <t>7.7</t>
   </si>
 </sst>
 </file>
@@ -475,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -490,6 +601,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -826,8 +938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:L34"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:B34"/>
+    <sheetView zoomScale="111" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1186,23 +1298,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397EBCE6-CC1A-FD42-88C3-8A4D005A4FAA}">
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="4" width="11" style="10"/>
-    <col min="5" max="5" width="19.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="10"/>
-    <col min="7" max="7" width="29.83203125" style="10" customWidth="1"/>
-    <col min="8" max="16384" width="11" style="10"/>
+    <col min="1" max="1" width="11" style="10"/>
+    <col min="2" max="2" width="11.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="11" style="10"/>
+    <col min="9" max="9" width="29.83203125" style="10" customWidth="1"/>
+    <col min="10" max="16384" width="11" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>7</v>
       </c>
@@ -1210,17 +1325,22 @@
         <v>36</v>
       </c>
       <c r="C1" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="F1"/>
-    </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="G1" s="10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
@@ -1228,20 +1348,26 @@
         <v>37</v>
       </c>
       <c r="C2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="12">
-        <v>7</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2"/>
-      <c r="G2" s="12" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F2" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="14"/>
+      <c r="I2" s="12" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
@@ -1249,17 +1375,23 @@
         <v>38</v>
       </c>
       <c r="C3" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D3" s="12">
-        <v>7</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3"/>
-    </row>
-    <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F3" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="14"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="10" t="s">
         <v>10</v>
       </c>
@@ -1267,17 +1399,22 @@
         <v>39</v>
       </c>
       <c r="C4" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D4" s="10">
-        <v>7</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4"/>
-    </row>
-    <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F4" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="10" t="s">
         <v>11</v>
       </c>
@@ -1285,17 +1422,22 @@
         <v>40</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D5" s="10">
-        <v>7</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="F5"/>
-    </row>
-    <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F5" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
@@ -1303,17 +1445,22 @@
         <v>41</v>
       </c>
       <c r="C6" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="10">
-        <v>7</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="F6"/>
-    </row>
-    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F6" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>13</v>
       </c>
@@ -1321,17 +1468,22 @@
         <v>42</v>
       </c>
       <c r="C7" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="12">
-        <v>7</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="F7"/>
-    </row>
-    <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F7" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="10" t="s">
         <v>14</v>
       </c>
@@ -1339,17 +1491,22 @@
         <v>43</v>
       </c>
       <c r="C8" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="D8" s="10">
-        <v>7</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8"/>
-    </row>
-    <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F8" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>15</v>
       </c>
@@ -1357,17 +1514,22 @@
         <v>44</v>
       </c>
       <c r="C9" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="D9" s="12">
-        <v>7</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9"/>
-    </row>
-    <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="F9" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="10" t="s">
         <v>16</v>
       </c>
@@ -1375,143 +1537,183 @@
         <v>45</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="10">
-        <v>8</v>
+        <v>75</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>110</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10"/>
-    </row>
-    <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D11" s="12">
-        <v>8</v>
-      </c>
-      <c r="E11" s="12" t="s">
+      <c r="C11" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="F11"/>
-    </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="D11" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A12" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D12" s="10">
-        <v>8</v>
-      </c>
-      <c r="E12" s="10" t="s">
+      <c r="C12" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F12"/>
-    </row>
-    <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="D12" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
         <v>19</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D13" s="12">
-        <v>8</v>
-      </c>
-      <c r="E13" s="12" t="s">
+      <c r="C13" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="F13"/>
-    </row>
-    <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="D13" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A14" s="12" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D14" s="12">
-        <v>8</v>
-      </c>
-      <c r="E14" s="12" t="s">
+      <c r="C14" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="F14"/>
-    </row>
-    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="D14" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A15" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D15" s="10">
-        <v>8</v>
-      </c>
-      <c r="E15" s="10" t="s">
+      <c r="C15" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="F15"/>
-    </row>
-    <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="D15" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
         <v>22</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C16" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" s="12">
-        <v>8</v>
-      </c>
-      <c r="E16" s="12" t="s">
+      <c r="C16" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="F16"/>
-    </row>
-    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="D16" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17" s="10" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C17" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="10">
-        <v>8</v>
-      </c>
-      <c r="E17" s="10" t="s">
+      <c r="C17" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="F17"/>
-    </row>
-    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="D17" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18" s="10" t="s">
         <v>24</v>
       </c>
@@ -1519,17 +1721,22 @@
         <v>53</v>
       </c>
       <c r="C18" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D18" s="10">
-        <v>7</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="F18"/>
-    </row>
-    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F18" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19" s="12" t="s">
         <v>25</v>
       </c>
@@ -1537,17 +1744,22 @@
         <v>54</v>
       </c>
       <c r="C19" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="E19" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="12">
-        <v>7</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="F19"/>
-    </row>
-    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F19" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20" s="10" t="s">
         <v>26</v>
       </c>
@@ -1555,17 +1767,22 @@
         <v>55</v>
       </c>
       <c r="C20" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="10">
-        <v>7</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="F20"/>
-    </row>
-    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F20" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21" s="12" t="s">
         <v>27</v>
       </c>
@@ -1573,17 +1790,22 @@
         <v>56</v>
       </c>
       <c r="C21" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="E21" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="12">
-        <v>7</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="F21"/>
-    </row>
-    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F21" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
         <v>28</v>
       </c>
@@ -1591,17 +1813,22 @@
         <v>57</v>
       </c>
       <c r="C22" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D22" s="12">
-        <v>7</v>
-      </c>
-      <c r="E22" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22"/>
-    </row>
-    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F22" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23" s="10" t="s">
         <v>29</v>
       </c>
@@ -1609,17 +1836,22 @@
         <v>58</v>
       </c>
       <c r="C23" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="D23" s="10">
-        <v>7</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F23"/>
-    </row>
-    <row r="24" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F23" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="s">
         <v>30</v>
       </c>
@@ -1627,17 +1859,22 @@
         <v>59</v>
       </c>
       <c r="C24" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E24" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="D24" s="12">
-        <v>7</v>
-      </c>
-      <c r="E24" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="F24"/>
-    </row>
-    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="F24" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25" s="12" t="s">
         <v>31</v>
       </c>
@@ -1645,17 +1882,22 @@
         <v>60</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" s="12">
-        <v>8</v>
+        <v>90</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>125</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="F25"/>
-    </row>
-    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26" s="12" t="s">
         <v>32</v>
       </c>
@@ -1663,17 +1905,22 @@
         <v>61</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D26" s="12">
-        <v>8</v>
+        <v>91</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>126</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="F26"/>
-    </row>
-    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27" s="10" t="s">
         <v>33</v>
       </c>
@@ -1681,17 +1928,22 @@
         <v>62</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="D27" s="10">
-        <v>8</v>
+        <v>92</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>127</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="F27"/>
-    </row>
-    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28" s="12" t="s">
         <v>34</v>
       </c>
@@ -1699,17 +1951,22 @@
         <v>63</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D28" s="12">
-        <v>8</v>
+        <v>93</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>128</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>93</v>
-      </c>
-      <c r="F28"/>
-    </row>
-    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29" s="12" t="s">
         <v>35</v>
       </c>
@@ -1717,38 +1974,53 @@
         <v>64</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="D29" s="12">
-        <v>8</v>
+        <v>94</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>129</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="F29"/>
-    </row>
-    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="E30"/>
-      <c r="F30"/>
-    </row>
-    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="E31"/>
-      <c r="F31"/>
-    </row>
-    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="E32"/>
-      <c r="F32"/>
-    </row>
-    <row r="33" spans="5:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="E33"/>
-      <c r="F33"/>
-    </row>
-    <row r="34" spans="5:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="E34"/>
-      <c r="F34"/>
+        <v>97</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+    </row>
+    <row r="31" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+    </row>
+    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+    </row>
+    <row r="33" spans="3:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+    </row>
+    <row r="34" spans="3:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="G34"/>
+      <c r="H34"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>